<commit_message>
Add notebook and note controllers
</commit_message>
<xml_diff>
--- a/enote-api-map.xlsx
+++ b/enote-api-map.xlsx
@@ -1,160 +1,231 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="Calc"/>
+  <workbookPr backupFile="false" showObjects="all" date1904="false"/>
+  <workbookProtection/>
+  <bookViews>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="990" firstSheet="0" activeTab="0"/>
+  </bookViews>
   <sheets>
-    <sheet state="visible" name="Лист1" sheetId="1" r:id="rId3"/>
+    <sheet name="Лист1" sheetId="1" state="visible" r:id="rId2"/>
   </sheets>
-  <definedNames/>
-  <calcPr/>
+  <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
+  <extLst>
+    <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
+      <loext:extCalcPr stringRefSyntax="CalcA1ExcelA1"/>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="28">
   <si>
-    <t>URL Path</t>
-  </si>
-  <si>
-    <t>Request method</t>
-  </si>
-  <si>
-    <t>Result</t>
-  </si>
-  <si>
-    <t>/users</t>
-  </si>
-  <si>
-    <t>GET</t>
-  </si>
-  <si>
-    <t>Get list of all users</t>
-  </si>
-  <si>
-    <t>POST</t>
-  </si>
-  <si>
-    <t>Create new users</t>
-  </si>
-  <si>
-    <t>/users/{userId}</t>
-  </si>
-  <si>
-    <t>Get user with {userId}</t>
-  </si>
-  <si>
-    <t>PUT</t>
-  </si>
-  <si>
-    <t>Update user with {userId}</t>
-  </si>
-  <si>
-    <t>DELETE</t>
-  </si>
-  <si>
-    <t>Delete user with {userId}</t>
-  </si>
-  <si>
-    <t>/users/{userId}/notebooks</t>
+    <t xml:space="preserve">URL Path</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Request method</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Result</t>
+  </si>
+  <si>
+    <t xml:space="preserve">/users</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GET</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Get list of all users</t>
+  </si>
+  <si>
+    <t xml:space="preserve">POST</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Create new user</t>
+  </si>
+  <si>
+    <t xml:space="preserve">/users/{userId}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Get user with {userId}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PUT</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Update user with {userId}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DELETE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Delete user with {userId}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">/users/{userId}/notebooks</t>
   </si>
   <si>
     <t xml:space="preserve">Get list of all [user with {userId}] notebooks </t>
   </si>
   <si>
-    <t>Create new [user with {userId}] notebooks</t>
-  </si>
-  <si>
-    <t>/users/{userId}/notebooks/{notebookId}</t>
-  </si>
-  <si>
-    <t>Get [user with {userId}] notebook with {notebookId}</t>
-  </si>
-  <si>
-    <t>Update [user with {userId}] notebook with {notebookId}</t>
-  </si>
-  <si>
-    <t>Delete [user with {userId}] notebook with {notebookId}</t>
-  </si>
-  <si>
-    <t>/users/{userId}/notebooks/{notebookId}/notes</t>
-  </si>
-  <si>
-    <t>Get list of all [user with {userId} and notebook with {notebookId}] notes</t>
-  </si>
-  <si>
-    <t>Create new [user with {userId} and notebook with {notebookId}] notes</t>
-  </si>
-  <si>
-    <t>/users/{userId}/notebooks/{notebookId}/notes/{noteId}</t>
-  </si>
-  <si>
-    <t>Get [user with {userId} and notebook with {notebookId}] note with {noteId}</t>
-  </si>
-  <si>
-    <t>Update [user with {userId} and notebook with {notebookId}] note with {noteId}</t>
-  </si>
-  <si>
-    <t>Delete [user with {userId} and notebook with {notebookId}] note with {noteId}</t>
+    <t xml:space="preserve">Create new [user with {userId}] notebook</t>
+  </si>
+  <si>
+    <t xml:space="preserve">/users/{userId}/notebooks/{notebookId}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Get [user with {userId}] notebook with {notebookId}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Update [user with {userId}] notebook with {notebookId}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Delete [user with {userId}] notebook with {notebookId}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">/users/{userId}/notebooks/{notebookId}/notes</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Get list of all [user with {userId} and notebook with {notebookId}] notes</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Create new [user with {userId} and notebook with {notebookId}] note</t>
+  </si>
+  <si>
+    <t xml:space="preserve">/users/{userId}/notebooks/{notebookId}/notes/{noteId}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Get [user with {userId} and notebook with {notebookId}] note with {noteId}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Update [user with {userId} and notebook with {notebookId}] note with {noteId}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Delete [user with {userId} and notebook with {notebookId}] note with {noteId}</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="General"/>
+  </numFmts>
+  <fonts count="5">
     <font>
-      <sz val="10.0"/>
+      <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
     </font>
-    <font/>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="0"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="0"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="0"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Cambria"/>
+      <family val="1"/>
+      <charset val="1"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
-      <patternFill patternType="lightGray"/>
+      <patternFill patternType="gray125"/>
     </fill>
   </fills>
   <borders count="1">
-    <border/>
+    <border diagonalUp="false" diagonalDown="false">
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
+  <cellStyleXfs count="20">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="41" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
   <cellXfs count="2">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
-  <cellStyles count="1">
-    <cellStyle xfId="0" name="Normal" builtinId="0"/>
+  <cellStyles count="6">
+    <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="false"/>
+    <cellStyle name="Comma" xfId="15" builtinId="3" customBuiltin="false"/>
+    <cellStyle name="Comma [0]" xfId="16" builtinId="6" customBuiltin="false"/>
+    <cellStyle name="Currency" xfId="17" builtinId="4" customBuiltin="false"/>
+    <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
+    <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
   </cellStyles>
-  <dxfs count="0"/>
 </styleSheet>
 </file>
 
-<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram"/>
-</file>
-
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:C16"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C18" activeCellId="0" sqref="C18"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultRowHeight="15.75"/>
   <cols>
-    <col customWidth="1" min="1" max="1" width="48.71"/>
-    <col customWidth="1" min="2" max="2" width="26.86"/>
-    <col customWidth="1" min="3" max="3" width="91.86"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="48.1938775510204"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="26.4591836734694"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="90.8469387755102"/>
+    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="14.1734693877551"/>
   </cols>
   <sheetData>
-    <row r="1">
+    <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -165,7 +236,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2">
+    <row r="2" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
         <v>3</v>
       </c>
@@ -176,7 +247,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3">
+    <row r="3" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
         <v>3</v>
       </c>
@@ -187,7 +258,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="4">
+    <row r="4" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
         <v>8</v>
       </c>
@@ -198,7 +269,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="5">
+    <row r="5" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
         <v>8</v>
       </c>
@@ -209,7 +280,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="6">
+    <row r="6" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
         <v>8</v>
       </c>
@@ -220,7 +291,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="7">
+    <row r="7" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="s">
         <v>14</v>
       </c>
@@ -231,7 +302,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="8">
+    <row r="8" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="1" t="s">
         <v>14</v>
       </c>
@@ -242,7 +313,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="9">
+    <row r="9" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="1" t="s">
         <v>17</v>
       </c>
@@ -253,7 +324,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="10">
+    <row r="10" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="1" t="s">
         <v>17</v>
       </c>
@@ -264,7 +335,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="11">
+    <row r="11" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="1" t="s">
         <v>17</v>
       </c>
@@ -275,7 +346,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="12">
+    <row r="12" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="1" t="s">
         <v>21</v>
       </c>
@@ -286,7 +357,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="13">
+    <row r="13" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="1" t="s">
         <v>21</v>
       </c>
@@ -297,7 +368,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="14">
+    <row r="14" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="1" t="s">
         <v>24</v>
       </c>
@@ -308,7 +379,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="15">
+    <row r="15" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="1" t="s">
         <v>24</v>
       </c>
@@ -319,7 +390,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="16">
+    <row r="16" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="1" t="s">
         <v>24</v>
       </c>
@@ -331,6 +402,12 @@
       </c>
     </row>
   </sheetData>
-  <drawing r:id="rId1"/>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.747916666666667" right="0.747916666666667" top="0.984027777777778" bottom="0.984027777777778" header="0.511805555555555" footer="0.511805555555555"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader/>
+    <oddFooter/>
+  </headerFooter>
 </worksheet>
 </file>
</xml_diff>